<commit_message>
rerun full analysis, update outputs
</commit_message>
<xml_diff>
--- a/output/Restab_D62_NTCnoRAPA_noDIFF_RAPA.xlsx
+++ b/output/Restab_D62_NTCnoRAPA_noDIFF_RAPA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="600">
   <si>
     <t xml:space="preserve">entrezgene</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">6202</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS8</t>
+  </si>
+  <si>
     <t xml:space="preserve">8503</t>
   </si>
   <si>
@@ -116,6 +119,9 @@
     <t xml:space="preserve">6125</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL5</t>
+  </si>
+  <si>
     <t xml:space="preserve">1301</t>
   </si>
   <si>
@@ -305,6 +311,9 @@
     <t xml:space="preserve">6157</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL27A</t>
+  </si>
+  <si>
     <t xml:space="preserve">10335</t>
   </si>
   <si>
@@ -368,6 +377,9 @@
     <t xml:space="preserve">114908</t>
   </si>
   <si>
+    <t xml:space="preserve">TMEM123</t>
+  </si>
+  <si>
     <t xml:space="preserve">1410</t>
   </si>
   <si>
@@ -461,6 +473,9 @@
     <t xml:space="preserve">10376</t>
   </si>
   <si>
+    <t xml:space="preserve">TUBA1B</t>
+  </si>
+  <si>
     <t xml:space="preserve">7846</t>
   </si>
   <si>
@@ -488,6 +503,9 @@
     <t xml:space="preserve">84324</t>
   </si>
   <si>
+    <t xml:space="preserve">SARNP</t>
+  </si>
+  <si>
     <t xml:space="preserve">23344</t>
   </si>
   <si>
@@ -596,6 +614,9 @@
     <t xml:space="preserve">10278</t>
   </si>
   <si>
+    <t xml:space="preserve">EFS</t>
+  </si>
+  <si>
     <t xml:space="preserve">9985</t>
   </si>
   <si>
@@ -641,6 +662,9 @@
     <t xml:space="preserve">51065</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS27L</t>
+  </si>
+  <si>
     <t xml:space="preserve">57611</t>
   </si>
   <si>
@@ -668,6 +692,9 @@
     <t xml:space="preserve">7023</t>
   </si>
   <si>
+    <t xml:space="preserve">TFAP4</t>
+  </si>
+  <si>
     <t xml:space="preserve">2013</t>
   </si>
   <si>
@@ -734,6 +761,9 @@
     <t xml:space="preserve">9953</t>
   </si>
   <si>
+    <t xml:space="preserve">HS3ST3B1</t>
+  </si>
+  <si>
     <t xml:space="preserve">256302</t>
   </si>
   <si>
@@ -761,6 +791,9 @@
     <t xml:space="preserve">27092</t>
   </si>
   <si>
+    <t xml:space="preserve">CACNG4</t>
+  </si>
+  <si>
     <t xml:space="preserve">23580</t>
   </si>
   <si>
@@ -788,6 +821,9 @@
     <t xml:space="preserve">283991</t>
   </si>
   <si>
+    <t xml:space="preserve">UBALD2</t>
+  </si>
+  <si>
     <t xml:space="preserve">146664</t>
   </si>
   <si>
@@ -935,6 +971,9 @@
     <t xml:space="preserve">29997</t>
   </si>
   <si>
+    <t xml:space="preserve">NOP53</t>
+  </si>
+  <si>
     <t xml:space="preserve">2014</t>
   </si>
   <si>
@@ -968,6 +1007,9 @@
     <t xml:space="preserve">151354</t>
   </si>
   <si>
+    <t xml:space="preserve">LRATD1</t>
+  </si>
+  <si>
     <t xml:space="preserve">81553</t>
   </si>
   <si>
@@ -977,6 +1019,9 @@
     <t xml:space="preserve">91461</t>
   </si>
   <si>
+    <t xml:space="preserve">PKDCC</t>
+  </si>
+  <si>
     <t xml:space="preserve">23433</t>
   </si>
   <si>
@@ -1040,6 +1085,9 @@
     <t xml:space="preserve">165215</t>
   </si>
   <si>
+    <t xml:space="preserve">FAM171B</t>
+  </si>
+  <si>
     <t xml:space="preserve">3329</t>
   </si>
   <si>
@@ -1061,6 +1109,9 @@
     <t xml:space="preserve">7857</t>
   </si>
   <si>
+    <t xml:space="preserve">SCG2</t>
+  </si>
+  <si>
     <t xml:space="preserve">81618</t>
   </si>
   <si>
@@ -1361,6 +1412,9 @@
     <t xml:space="preserve">85027</t>
   </si>
   <si>
+    <t xml:space="preserve">SMIM3</t>
+  </si>
+  <si>
     <t xml:space="preserve">10569</t>
   </si>
   <si>
@@ -1454,9 +1508,6 @@
     <t xml:space="preserve">2970</t>
   </si>
   <si>
-    <t xml:space="preserve">GTF2IP1</t>
-  </si>
-  <si>
     <t xml:space="preserve">2791</t>
   </si>
   <si>
@@ -1478,9 +1529,15 @@
     <t xml:space="preserve">25798</t>
   </si>
   <si>
+    <t xml:space="preserve">BRI3</t>
+  </si>
+  <si>
     <t xml:space="preserve">11333</t>
   </si>
   <si>
+    <t xml:space="preserve">PDAP1</t>
+  </si>
+  <si>
     <t xml:space="preserve">5054</t>
   </si>
   <si>
@@ -1556,6 +1613,9 @@
     <t xml:space="preserve">55893</t>
   </si>
   <si>
+    <t xml:space="preserve">ZNF395</t>
+  </si>
+  <si>
     <t xml:space="preserve">5327</t>
   </si>
   <si>
@@ -1649,6 +1709,9 @@
     <t xml:space="preserve">9568</t>
   </si>
   <si>
+    <t xml:space="preserve">GABBR2</t>
+  </si>
+  <si>
     <t xml:space="preserve">114299</t>
   </si>
   <si>
@@ -1700,6 +1763,9 @@
     <t xml:space="preserve">6303</t>
   </si>
   <si>
+    <t xml:space="preserve">SAT1</t>
+  </si>
+  <si>
     <t xml:space="preserve">8406</t>
   </si>
   <si>
@@ -1713,6 +1779,9 @@
   </si>
   <si>
     <t xml:space="preserve">6191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS4X</t>
   </si>
   <si>
     <t xml:space="preserve">56062</t>
@@ -2258,7 +2327,9 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" t="n">
         <v>-0.275317419828105</v>
       </c>
@@ -2274,10 +2345,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="n">
         <v>1.57604101828909</v>
@@ -2294,10 +2365,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="n">
         <v>1.71767650810491</v>
@@ -2314,10 +2385,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="n">
         <v>-1.04785126363008</v>
@@ -2334,10 +2405,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" t="n">
         <v>1.40203134123372</v>
@@ -2354,10 +2425,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" t="n">
         <v>3.90619626658478</v>
@@ -2374,9 +2445,11 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16"/>
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
       <c r="C16" t="n">
         <v>-0.682816063075055</v>
       </c>
@@ -2392,10 +2465,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" t="n">
         <v>0.8562904081752</v>
@@ -2412,10 +2485,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" t="n">
         <v>1.91949371668405</v>
@@ -2432,10 +2505,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="n">
         <v>-1.12703216518943</v>
@@ -2452,10 +2525,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" t="n">
         <v>0.753475594553754</v>
@@ -2472,10 +2545,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" t="n">
         <v>-0.463430417369665</v>
@@ -2492,10 +2565,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" t="n">
         <v>0.707257077673417</v>
@@ -2512,10 +2585,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" t="n">
         <v>0.942174899672789</v>
@@ -2532,10 +2605,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" t="n">
         <v>-2.37119368662972</v>
@@ -2552,10 +2625,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" t="n">
         <v>0.487523655411476</v>
@@ -2572,10 +2645,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" t="n">
         <v>1.13117925435868</v>
@@ -2592,10 +2665,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" t="n">
         <v>2.04575507346853</v>
@@ -2612,10 +2685,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" t="n">
         <v>0.619775806389201</v>
@@ -2632,10 +2705,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" t="n">
         <v>1.57321933824552</v>
@@ -2652,10 +2725,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" t="n">
         <v>-0.539020986907587</v>
@@ -2672,10 +2745,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" t="n">
         <v>0.807249349488872</v>
@@ -2692,10 +2765,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" t="n">
         <v>-1.50163084221261</v>
@@ -2712,10 +2785,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" t="n">
         <v>-0.593241821141259</v>
@@ -2732,10 +2805,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" t="n">
         <v>-0.941701069065171</v>
@@ -2752,10 +2825,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" t="n">
         <v>0.816332371237823</v>
@@ -2772,10 +2845,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C36" t="n">
         <v>1.91273475590912</v>
@@ -2792,10 +2865,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C37" t="n">
         <v>0.734955038333417</v>
@@ -2812,10 +2885,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" t="n">
         <v>-0.543132617315906</v>
@@ -2832,10 +2905,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" t="n">
         <v>1.22581866854015</v>
@@ -2852,10 +2925,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" t="n">
         <v>1.22741804906831</v>
@@ -2872,10 +2945,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" t="n">
         <v>-1.34852431225236</v>
@@ -2892,10 +2965,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C42" t="n">
         <v>-0.73828735852067</v>
@@ -2912,10 +2985,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C43" t="n">
         <v>-1.98562044896721</v>
@@ -2932,10 +3005,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C44" t="n">
         <v>-0.516441024540608</v>
@@ -2952,10 +3025,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C45" t="n">
         <v>0.767134982753178</v>
@@ -2972,10 +3045,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C46" t="n">
         <v>-0.54809346670868</v>
@@ -2992,10 +3065,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C47" t="n">
         <v>-2.57973554571366</v>
@@ -3012,9 +3085,11 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48"/>
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>99</v>
+      </c>
       <c r="C48" t="n">
         <v>-0.379331034625178</v>
       </c>
@@ -3030,10 +3105,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C49" t="n">
         <v>1.78773204194994</v>
@@ -3050,10 +3125,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C50" t="n">
         <v>-0.843688735295881</v>
@@ -3070,10 +3145,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C51" t="n">
         <v>0.981265416448113</v>
@@ -3090,10 +3165,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C52" t="n">
         <v>0.779404598302324</v>
@@ -3110,10 +3185,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C53" t="n">
         <v>0.749630521491336</v>
@@ -3130,10 +3205,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C54" t="n">
         <v>2.14369791853373</v>
@@ -3150,10 +3225,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C55" t="n">
         <v>-0.761291767390058</v>
@@ -3170,10 +3245,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C56" t="n">
         <v>0.443062334066894</v>
@@ -3190,10 +3265,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C57" t="n">
         <v>1.23482347456558</v>
@@ -3210,10 +3285,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C58" t="n">
         <v>1.56301598543085</v>
@@ -3230,9 +3305,11 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59"/>
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
       <c r="C59" t="n">
         <v>-0.854319932225181</v>
       </c>
@@ -3248,10 +3325,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C60" t="n">
         <v>0.741932317817046</v>
@@ -3268,10 +3345,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C61" t="n">
         <v>0.542635019264903</v>
@@ -3288,10 +3365,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C62" t="n">
         <v>-0.506750787360335</v>
@@ -3308,10 +3385,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C63" t="n">
         <v>1.64316288048163</v>
@@ -3328,10 +3405,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C64" t="n">
         <v>-3.78292657316219</v>
@@ -3348,10 +3425,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C65" t="n">
         <v>-3.72480638253509</v>
@@ -3368,10 +3445,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C66" t="n">
         <v>-7.93664835425211</v>
@@ -3388,10 +3465,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C67" t="n">
         <v>-0.559796157587176</v>
@@ -3408,10 +3485,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C68" t="n">
         <v>0.893470055291608</v>
@@ -3428,10 +3505,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C69" t="n">
         <v>-0.679904650228545</v>
@@ -3448,10 +3525,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C70" t="n">
         <v>4.81202633277723</v>
@@ -3468,10 +3545,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C71" t="n">
         <v>-1.49494054583733</v>
@@ -3488,10 +3565,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C72" t="n">
         <v>2.00804947520879</v>
@@ -3508,10 +3585,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C73" t="n">
         <v>2.47049598007241</v>
@@ -3528,10 +3605,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C74" t="n">
         <v>-1.7108194770765</v>
@@ -3548,9 +3625,11 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75"/>
+        <v>152</v>
+      </c>
+      <c r="B75" t="s">
+        <v>153</v>
+      </c>
       <c r="C75" t="n">
         <v>0.688924967787424</v>
       </c>
@@ -3566,10 +3645,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C76" t="n">
         <v>0.832623083770608</v>
@@ -3586,10 +3665,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C77" t="n">
         <v>1.11622512684714</v>
@@ -3606,10 +3685,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C78" t="n">
         <v>-0.528098844977356</v>
@@ -3626,10 +3705,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C79" t="n">
         <v>-0.88045452417194</v>
@@ -3646,9 +3725,11 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80"/>
+        <v>162</v>
+      </c>
+      <c r="B80" t="s">
+        <v>163</v>
+      </c>
       <c r="C80" t="n">
         <v>1.41412601331546</v>
       </c>
@@ -3664,10 +3745,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C81" t="n">
         <v>0.914552695133569</v>
@@ -3684,10 +3765,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C82" t="n">
         <v>-0.361930247030631</v>
@@ -3704,10 +3785,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B83" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C83" t="n">
         <v>1.18821593076913</v>
@@ -3724,10 +3805,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C84" t="n">
         <v>1.71092305249683</v>
@@ -3744,10 +3825,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C85" t="n">
         <v>-0.545806787730398</v>
@@ -3764,10 +3845,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C86" t="n">
         <v>-1.13589068313873</v>
@@ -3784,10 +3865,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C87" t="n">
         <v>-0.816337918102552</v>
@@ -3804,10 +3885,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C88" t="n">
         <v>-0.403513146154267</v>
@@ -3824,10 +3905,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C89" t="n">
         <v>-0.468289026939251</v>
@@ -3844,10 +3925,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B90" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C90" t="n">
         <v>1.29395120720687</v>
@@ -3864,10 +3945,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C91" t="n">
         <v>8.88026853312092</v>
@@ -3884,10 +3965,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C92" t="n">
         <v>0.595526965536351</v>
@@ -3904,10 +3985,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C93" t="n">
         <v>-0.579360296178417</v>
@@ -3924,10 +4005,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C94" t="n">
         <v>-1.93716433334258</v>
@@ -3944,10 +4025,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C95" t="n">
         <v>1.12012554350237</v>
@@ -3964,10 +4045,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C96" t="n">
         <v>1.92986774050221</v>
@@ -3984,10 +4065,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B97" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C97" t="n">
         <v>1.81557045772487</v>
@@ -4004,7 +4085,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B98"/>
       <c r="C98" t="n">
@@ -4022,9 +4103,11 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>193</v>
-      </c>
-      <c r="B99"/>
+        <v>199</v>
+      </c>
+      <c r="B99" t="s">
+        <v>200</v>
+      </c>
       <c r="C99" t="n">
         <v>1.59479690745682</v>
       </c>
@@ -4040,10 +4123,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C100" t="n">
         <v>1.52324296814115</v>
@@ -4060,10 +4143,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C101" t="n">
         <v>-2.85393147744944</v>
@@ -4080,10 +4163,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C102" t="n">
         <v>1.06672232604748</v>
@@ -4100,10 +4183,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C103" t="n">
         <v>0.430464988208846</v>
@@ -4120,10 +4203,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C104" t="n">
         <v>0.909757025782293</v>
@@ -4140,10 +4223,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C105" t="n">
         <v>1.73724158497009</v>
@@ -4160,10 +4243,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C106" t="n">
         <v>0.898148632546458</v>
@@ -4180,9 +4263,11 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>208</v>
-      </c>
-      <c r="B107"/>
+        <v>215</v>
+      </c>
+      <c r="B107" t="s">
+        <v>216</v>
+      </c>
       <c r="C107" t="n">
         <v>0.421437128849645</v>
       </c>
@@ -4198,10 +4283,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B108" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C108" t="n">
         <v>-1.55513811184231</v>
@@ -4218,10 +4303,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B109" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C109" t="n">
         <v>1.11265798103263</v>
@@ -4238,10 +4323,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C110" t="n">
         <v>-0.674350800508459</v>
@@ -4258,10 +4343,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C111" t="n">
         <v>1.38364629962279</v>
@@ -4278,9 +4363,11 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>217</v>
-      </c>
-      <c r="B112"/>
+        <v>225</v>
+      </c>
+      <c r="B112" t="s">
+        <v>226</v>
+      </c>
       <c r="C112" t="n">
         <v>-2.10334291717082</v>
       </c>
@@ -4296,10 +4383,10 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B113" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C113" t="n">
         <v>-1.35643445731739</v>
@@ -4316,10 +4403,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C114" t="n">
         <v>-0.570822786892494</v>
@@ -4336,10 +4423,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C115" t="n">
         <v>2.78629164703604</v>
@@ -4356,10 +4443,10 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C116" t="n">
         <v>-1.24753748023059</v>
@@ -4376,7 +4463,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B117"/>
       <c r="C117" t="n">
@@ -4394,10 +4481,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B118" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C118" t="n">
         <v>-0.963859645865659</v>
@@ -4414,10 +4501,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B119" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C119" t="n">
         <v>0.672666174255338</v>
@@ -4434,10 +4521,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B120" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C120" t="n">
         <v>0.337171545639972</v>
@@ -4454,10 +4541,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B121" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C121" t="n">
         <v>1.37410196314489</v>
@@ -4474,10 +4561,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B122" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C122" t="n">
         <v>-0.491822405115355</v>
@@ -4494,10 +4581,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B123" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C123" t="n">
         <v>1.28396645607104</v>
@@ -4514,9 +4601,11 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>239</v>
-      </c>
-      <c r="B124"/>
+        <v>248</v>
+      </c>
+      <c r="B124" t="s">
+        <v>249</v>
+      </c>
       <c r="C124" t="n">
         <v>-0.997366768528037</v>
       </c>
@@ -4532,10 +4621,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="C125" t="n">
         <v>-1.26283943812901</v>
@@ -4552,10 +4641,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B126" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="C126" t="n">
         <v>0.922102138241602</v>
@@ -4572,10 +4661,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="B127" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="C127" t="n">
         <v>1.04164577397254</v>
@@ -4592,10 +4681,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C128" t="n">
         <v>-0.512995929777985</v>
@@ -4612,9 +4701,11 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>248</v>
-      </c>
-      <c r="B129"/>
+        <v>258</v>
+      </c>
+      <c r="B129" t="s">
+        <v>259</v>
+      </c>
       <c r="C129" t="n">
         <v>-0.667690068000753</v>
       </c>
@@ -4630,10 +4721,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B130" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C130" t="n">
         <v>0.668518980843622</v>
@@ -4650,10 +4741,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="B131" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="C131" t="n">
         <v>-1.38020600466825</v>
@@ -4670,10 +4761,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="B132" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C132" t="n">
         <v>0.494453723479677</v>
@@ -4690,10 +4781,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="B133" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="C133" t="n">
         <v>6.92882618455984</v>
@@ -4710,9 +4801,11 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>257</v>
-      </c>
-      <c r="B134"/>
+        <v>268</v>
+      </c>
+      <c r="B134" t="s">
+        <v>269</v>
+      </c>
       <c r="C134" t="n">
         <v>-0.711926604615854</v>
       </c>
@@ -4728,10 +4821,10 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B135" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="C135" t="n">
         <v>-2.523447740588</v>
@@ -4748,10 +4841,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B136" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C136" t="n">
         <v>-0.913826929950955</v>
@@ -4768,10 +4861,10 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B137" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="C137" t="n">
         <v>-0.455164201051049</v>
@@ -4788,10 +4881,10 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B138" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C138" t="n">
         <v>0.913060300216635</v>
@@ -4808,10 +4901,10 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B139" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="C139" t="n">
         <v>-0.462089877350446</v>
@@ -4828,10 +4921,10 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B140" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C140" t="n">
         <v>0.982451624764548</v>
@@ -4848,10 +4941,10 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B141" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C141" t="n">
         <v>-0.579111381122436</v>
@@ -4868,10 +4961,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C142" t="n">
         <v>0.689445784931033</v>
@@ -4888,10 +4981,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B143" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="C143" t="n">
         <v>-2.08897923213421</v>
@@ -4908,10 +5001,10 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B144" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C144" t="n">
         <v>-0.611039442809241</v>
@@ -4928,10 +5021,10 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B145" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="C145" t="n">
         <v>-0.660903253871079</v>
@@ -4948,10 +5041,10 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B146" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="C146" t="n">
         <v>0.907964190163981</v>
@@ -4968,10 +5061,10 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="B147" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="C147" t="n">
         <v>-1.13066871927927</v>
@@ -4988,10 +5081,10 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B148" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="C148" t="n">
         <v>-0.438712610241186</v>
@@ -5008,10 +5101,10 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="B149" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="C149" t="n">
         <v>-0.795464457097999</v>
@@ -5028,10 +5121,10 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B150" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C150" t="n">
         <v>0.952193235869934</v>
@@ -5048,10 +5141,10 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="B151" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="C151" t="n">
         <v>0.801224508936476</v>
@@ -5068,10 +5161,10 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B152" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="C152" t="n">
         <v>0.455763655512034</v>
@@ -5088,10 +5181,10 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B153" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="C153" t="n">
         <v>-0.881153086396227</v>
@@ -5108,10 +5201,10 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B154" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="C154" t="n">
         <v>1.08868300753797</v>
@@ -5128,10 +5221,10 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B155" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="C155" t="n">
         <v>4.98366851868183</v>
@@ -5148,10 +5241,10 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="B156" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="C156" t="n">
         <v>1.12173407903948</v>
@@ -5168,10 +5261,10 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B157" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="C157" t="n">
         <v>1.42340662348032</v>
@@ -5188,10 +5281,10 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B158" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C158" t="n">
         <v>1.39597841431106</v>
@@ -5208,9 +5301,11 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>306</v>
-      </c>
-      <c r="B159"/>
+        <v>318</v>
+      </c>
+      <c r="B159" t="s">
+        <v>319</v>
+      </c>
       <c r="C159" t="n">
         <v>-0.423762186770283</v>
       </c>
@@ -5226,10 +5321,10 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="B160" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="C160" t="n">
         <v>1.65071683758571</v>
@@ -5246,10 +5341,10 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="B161" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="C161" t="n">
         <v>0.882573982529164</v>
@@ -5266,10 +5361,10 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="B162" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="C162" t="n">
         <v>-6.46179831376267</v>
@@ -5286,10 +5381,10 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="B163" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C163" t="n">
         <v>-0.841342943648951</v>
@@ -5306,10 +5401,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="B164" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="C164" t="n">
         <v>-0.565924962193767</v>
@@ -5326,9 +5421,11 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>317</v>
-      </c>
-      <c r="B165"/>
+        <v>330</v>
+      </c>
+      <c r="B165" t="s">
+        <v>331</v>
+      </c>
       <c r="C165" t="n">
         <v>1.21909683272916</v>
       </c>
@@ -5344,10 +5441,10 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="B166" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C166" t="n">
         <v>1.2878219155145</v>
@@ -5364,9 +5461,11 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>320</v>
-      </c>
-      <c r="B167"/>
+        <v>334</v>
+      </c>
+      <c r="B167" t="s">
+        <v>335</v>
+      </c>
       <c r="C167" t="n">
         <v>-0.682695557633659</v>
       </c>
@@ -5382,10 +5481,10 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="B168" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="C168" t="n">
         <v>0.804085159459172</v>
@@ -5402,10 +5501,10 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="B169" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="C169" t="n">
         <v>2.66935941724356</v>
@@ -5422,10 +5521,10 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="B170" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="C170" t="n">
         <v>-1.46886261154868</v>
@@ -5442,10 +5541,10 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="B171" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="C171" t="n">
         <v>0.934146207338607</v>
@@ -5462,10 +5561,10 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="B172" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="C172" t="n">
         <v>-0.689694257964865</v>
@@ -5482,10 +5581,10 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="B173" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="C173" t="n">
         <v>0.548866498914212</v>
@@ -5502,10 +5601,10 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="B174" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="C174" t="n">
         <v>-0.718014788331015</v>
@@ -5522,10 +5621,10 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="B175" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="C175" t="n">
         <v>0.728118049688987</v>
@@ -5542,10 +5641,10 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B176" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="C176" t="n">
         <v>1.45161925233552</v>
@@ -5562,10 +5661,10 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="B177" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="C177" t="n">
         <v>2.00805397204409</v>
@@ -5582,9 +5681,11 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>341</v>
-      </c>
-      <c r="B178"/>
+        <v>356</v>
+      </c>
+      <c r="B178" t="s">
+        <v>357</v>
+      </c>
       <c r="C178" t="n">
         <v>0.765521800414706</v>
       </c>
@@ -5600,10 +5701,10 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>342</v>
+        <v>358</v>
       </c>
       <c r="B179" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
       <c r="C179" t="n">
         <v>0.446880807699543</v>
@@ -5620,10 +5721,10 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="B180" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="C180" t="n">
         <v>0.645349144453083</v>
@@ -5640,10 +5741,10 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="B181" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C181" t="n">
         <v>-0.881978106027287</v>
@@ -5660,9 +5761,11 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>348</v>
-      </c>
-      <c r="B182"/>
+        <v>364</v>
+      </c>
+      <c r="B182" t="s">
+        <v>365</v>
+      </c>
       <c r="C182" t="n">
         <v>1.57953986788673</v>
       </c>
@@ -5678,10 +5781,10 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="B183" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="C183" t="n">
         <v>-1.15693751872385</v>
@@ -5698,10 +5801,10 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>351</v>
+        <v>368</v>
       </c>
       <c r="B184" t="s">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="C184" t="n">
         <v>0.636879336221171</v>
@@ -5718,10 +5821,10 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="B185" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
       <c r="C185" t="n">
         <v>0.541486302863484</v>
@@ -5738,10 +5841,10 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="B186" t="s">
-        <v>356</v>
+        <v>373</v>
       </c>
       <c r="C186" t="n">
         <v>-1.91575453006224</v>
@@ -5758,10 +5861,10 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>374</v>
       </c>
       <c r="B187" t="s">
-        <v>358</v>
+        <v>375</v>
       </c>
       <c r="C187" t="n">
         <v>3.24668583500271</v>
@@ -5778,10 +5881,10 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>359</v>
+        <v>376</v>
       </c>
       <c r="B188" t="s">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="C188" t="n">
         <v>0.784197126354124</v>
@@ -5798,10 +5901,10 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>361</v>
+        <v>378</v>
       </c>
       <c r="B189" t="s">
-        <v>362</v>
+        <v>379</v>
       </c>
       <c r="C189" t="n">
         <v>0.529917240075084</v>
@@ -5818,10 +5921,10 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="B190" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="C190" t="n">
         <v>-0.959127507153906</v>
@@ -5838,10 +5941,10 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>365</v>
+        <v>382</v>
       </c>
       <c r="B191" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
       <c r="C191" t="n">
         <v>2.14339655865055</v>
@@ -5858,10 +5961,10 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="B192" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="C192" t="n">
         <v>-0.383933600508747</v>
@@ -5878,10 +5981,10 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
       <c r="B193" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
       <c r="C193" t="n">
         <v>1.2706644252335</v>
@@ -5898,10 +6001,10 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
       <c r="B194" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="C194" t="n">
         <v>-1.391872421634</v>
@@ -5918,10 +6021,10 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="B195" t="s">
-        <v>374</v>
+        <v>391</v>
       </c>
       <c r="C195" t="n">
         <v>-0.506299282798707</v>
@@ -5938,10 +6041,10 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="B196" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="C196" t="n">
         <v>-0.388684470243017</v>
@@ -5958,10 +6061,10 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
       <c r="B197" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="C197" t="n">
         <v>-0.889841727512086</v>
@@ -5978,10 +6081,10 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
       <c r="B198" t="s">
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="C198" t="n">
         <v>-0.753190443785652</v>
@@ -5998,10 +6101,10 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="B199" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
       <c r="C199" t="n">
         <v>0.948772541512792</v>
@@ -6018,10 +6121,10 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="B200" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="C200" t="n">
         <v>0.687884607348519</v>
@@ -6038,10 +6141,10 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
       <c r="B201" t="s">
-        <v>386</v>
+        <v>403</v>
       </c>
       <c r="C201" t="n">
         <v>-0.935553966956327</v>
@@ -6058,7 +6161,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="B202"/>
       <c r="C202" t="n">
@@ -6076,10 +6179,10 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
       <c r="B203" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C203" t="n">
         <v>1.15345712662646</v>
@@ -6096,10 +6199,10 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="B204" t="s">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="C204" t="n">
         <v>1.85807491220989</v>
@@ -6116,10 +6219,10 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="B205" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
       <c r="C205" t="n">
         <v>0.805912758687395</v>
@@ -6136,10 +6239,10 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>394</v>
+        <v>411</v>
       </c>
       <c r="B206" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="C206" t="n">
         <v>2.74844131948508</v>
@@ -6156,10 +6259,10 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>396</v>
+        <v>413</v>
       </c>
       <c r="B207" t="s">
-        <v>397</v>
+        <v>414</v>
       </c>
       <c r="C207" t="n">
         <v>-0.495753535060664</v>
@@ -6176,10 +6279,10 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="B208" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="C208" t="n">
         <v>0.732345351651516</v>
@@ -6196,10 +6299,10 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="B209" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="C209" t="n">
         <v>-0.812682593245288</v>
@@ -6216,10 +6319,10 @@
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="B210" t="s">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="C210" t="n">
         <v>-0.588647121295813</v>
@@ -6236,10 +6339,10 @@
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>404</v>
+        <v>421</v>
       </c>
       <c r="B211" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="C211" t="n">
         <v>-3.09539619998189</v>
@@ -6256,10 +6359,10 @@
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="B212" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
       <c r="C212" t="n">
         <v>-0.358012953342949</v>
@@ -6276,10 +6379,10 @@
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="B213" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="C213" t="n">
         <v>-0.645085571054351</v>
@@ -6296,10 +6399,10 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="B214" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
       <c r="C214" t="n">
         <v>-0.520781637493295</v>
@@ -6316,10 +6419,10 @@
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>412</v>
+        <v>429</v>
       </c>
       <c r="B215" t="s">
-        <v>413</v>
+        <v>430</v>
       </c>
       <c r="C215" t="n">
         <v>-0.939224080761367</v>
@@ -6336,10 +6439,10 @@
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="B216" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
       <c r="C216" t="n">
         <v>1.15343797880589</v>
@@ -6356,10 +6459,10 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="B217" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="C217" t="n">
         <v>0.485181596619596</v>
@@ -6376,10 +6479,10 @@
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="B218" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="C218" t="n">
         <v>0.32722688012295</v>
@@ -6396,10 +6499,10 @@
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>420</v>
+        <v>437</v>
       </c>
       <c r="B219" t="s">
-        <v>421</v>
+        <v>438</v>
       </c>
       <c r="C219" t="n">
         <v>2.80871751054657</v>
@@ -6416,10 +6519,10 @@
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>422</v>
+        <v>439</v>
       </c>
       <c r="B220" t="s">
-        <v>423</v>
+        <v>440</v>
       </c>
       <c r="C220" t="n">
         <v>-0.432901687720035</v>
@@ -6436,10 +6539,10 @@
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
       <c r="B221" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="C221" t="n">
         <v>-1.50877023684672</v>
@@ -6456,10 +6559,10 @@
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="B222" t="s">
-        <v>427</v>
+        <v>444</v>
       </c>
       <c r="C222" t="n">
         <v>-2.21386233853972</v>
@@ -6476,10 +6579,10 @@
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>428</v>
+        <v>445</v>
       </c>
       <c r="B223" t="s">
-        <v>429</v>
+        <v>446</v>
       </c>
       <c r="C223" t="n">
         <v>-0.834055155457617</v>
@@ -6496,10 +6599,10 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>430</v>
+        <v>447</v>
       </c>
       <c r="B224" t="s">
-        <v>431</v>
+        <v>448</v>
       </c>
       <c r="C224" t="n">
         <v>0.789013558704083</v>
@@ -6516,10 +6619,10 @@
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="B225" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="C225" t="n">
         <v>-0.844468702864183</v>
@@ -6536,10 +6639,10 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="B226" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
       <c r="C226" t="n">
         <v>-0.48380386725187</v>
@@ -6556,10 +6659,10 @@
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>436</v>
+        <v>453</v>
       </c>
       <c r="B227" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="C227" t="n">
         <v>1.69851215259888</v>
@@ -6576,10 +6679,10 @@
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="B228" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="C228" t="n">
         <v>-1.42016560620637</v>
@@ -6596,10 +6699,10 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="B229" t="s">
-        <v>441</v>
+        <v>458</v>
       </c>
       <c r="C229" t="n">
         <v>1.61892676062892</v>
@@ -6616,10 +6719,10 @@
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="B230" t="s">
-        <v>443</v>
+        <v>460</v>
       </c>
       <c r="C230" t="n">
         <v>6.80552998661244</v>
@@ -6636,10 +6739,10 @@
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>444</v>
+        <v>461</v>
       </c>
       <c r="B231" t="s">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="C231" t="n">
         <v>-1.51458548920084</v>
@@ -6656,10 +6759,10 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>446</v>
+        <v>463</v>
       </c>
       <c r="B232" t="s">
-        <v>447</v>
+        <v>464</v>
       </c>
       <c r="C232" t="n">
         <v>1.68369294345315</v>
@@ -6676,9 +6779,11 @@
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>448</v>
-      </c>
-      <c r="B233"/>
+        <v>465</v>
+      </c>
+      <c r="B233" t="s">
+        <v>466</v>
+      </c>
       <c r="C233" t="n">
         <v>1.12327493400244</v>
       </c>
@@ -6694,10 +6799,10 @@
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="B234" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="C234" t="n">
         <v>-0.687841982640829</v>
@@ -6714,10 +6819,10 @@
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="B235" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
       <c r="C235" t="n">
         <v>-1.64712288543063</v>
@@ -6734,10 +6839,10 @@
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="B236" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="C236" t="n">
         <v>-1.41963137058807</v>
@@ -6754,10 +6859,10 @@
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="B237" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="C237" t="n">
         <v>5.87065416271673</v>
@@ -6774,10 +6879,10 @@
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
       <c r="B238" t="s">
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="C238" t="n">
         <v>1.37140552567137</v>
@@ -6794,10 +6899,10 @@
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="B239" t="s">
-        <v>460</v>
+        <v>478</v>
       </c>
       <c r="C239" t="n">
         <v>-0.608762743652672</v>
@@ -6814,10 +6919,10 @@
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>461</v>
+        <v>479</v>
       </c>
       <c r="B240" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="C240" t="n">
         <v>1.3849945819712</v>
@@ -6834,10 +6939,10 @@
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>463</v>
+        <v>481</v>
       </c>
       <c r="B241" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="C241" t="n">
         <v>-3.05187356407729</v>
@@ -6854,10 +6959,10 @@
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>465</v>
+        <v>483</v>
       </c>
       <c r="B242" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="C242" t="n">
         <v>-0.326598126530897</v>
@@ -6874,10 +6979,10 @@
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="B243" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
       <c r="C243" t="n">
         <v>-1.00116563025979</v>
@@ -6894,10 +6999,10 @@
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>469</v>
+        <v>487</v>
       </c>
       <c r="B244" t="s">
-        <v>470</v>
+        <v>488</v>
       </c>
       <c r="C244" t="n">
         <v>-1.64837508032265</v>
@@ -6914,10 +7019,10 @@
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>471</v>
+        <v>489</v>
       </c>
       <c r="B245" t="s">
-        <v>472</v>
+        <v>490</v>
       </c>
       <c r="C245" t="n">
         <v>-0.400525833731504</v>
@@ -6934,10 +7039,10 @@
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>473</v>
+        <v>491</v>
       </c>
       <c r="B246" t="s">
-        <v>474</v>
+        <v>492</v>
       </c>
       <c r="C246" t="n">
         <v>0.893677162918426</v>
@@ -6954,10 +7059,10 @@
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>475</v>
+        <v>493</v>
       </c>
       <c r="B247" t="s">
-        <v>476</v>
+        <v>494</v>
       </c>
       <c r="C247" t="n">
         <v>-0.967594377703446</v>
@@ -6974,10 +7079,10 @@
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>477</v>
+        <v>495</v>
       </c>
       <c r="B248" t="s">
-        <v>478</v>
+        <v>496</v>
       </c>
       <c r="C248" t="n">
         <v>-1.21564468526971</v>
@@ -6994,11 +7099,9 @@
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>479</v>
-      </c>
-      <c r="B249" t="s">
-        <v>480</v>
-      </c>
+        <v>497</v>
+      </c>
+      <c r="B249"/>
       <c r="C249" t="n">
         <v>0.562230199422059</v>
       </c>
@@ -7014,10 +7117,10 @@
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>481</v>
+        <v>498</v>
       </c>
       <c r="B250" t="s">
-        <v>482</v>
+        <v>499</v>
       </c>
       <c r="C250" t="n">
         <v>0.748007252952246</v>
@@ -7034,10 +7137,10 @@
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>483</v>
+        <v>500</v>
       </c>
       <c r="B251" t="s">
-        <v>484</v>
+        <v>501</v>
       </c>
       <c r="C251" t="n">
         <v>0.882755792445024</v>
@@ -7054,10 +7157,10 @@
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>485</v>
+        <v>502</v>
       </c>
       <c r="B252" t="s">
-        <v>486</v>
+        <v>503</v>
       </c>
       <c r="C252" t="n">
         <v>-2.15367899048276</v>
@@ -7074,9 +7177,11 @@
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>487</v>
-      </c>
-      <c r="B253"/>
+        <v>504</v>
+      </c>
+      <c r="B253" t="s">
+        <v>505</v>
+      </c>
       <c r="C253" t="n">
         <v>-0.552448366897736</v>
       </c>
@@ -7092,9 +7197,11 @@
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>488</v>
-      </c>
-      <c r="B254"/>
+        <v>506</v>
+      </c>
+      <c r="B254" t="s">
+        <v>507</v>
+      </c>
       <c r="C254" t="n">
         <v>0.644660904576836</v>
       </c>
@@ -7110,10 +7217,10 @@
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>489</v>
+        <v>508</v>
       </c>
       <c r="B255" t="s">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="C255" t="n">
         <v>-1.53762142728896</v>
@@ -7130,10 +7237,10 @@
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>491</v>
+        <v>510</v>
       </c>
       <c r="B256" t="s">
-        <v>492</v>
+        <v>511</v>
       </c>
       <c r="C256" t="n">
         <v>0.9465102957139</v>
@@ -7150,10 +7257,10 @@
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>493</v>
+        <v>512</v>
       </c>
       <c r="B257" t="s">
-        <v>494</v>
+        <v>513</v>
       </c>
       <c r="C257" t="n">
         <v>-0.674452046257205</v>
@@ -7170,10 +7277,10 @@
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>495</v>
+        <v>514</v>
       </c>
       <c r="B258" t="s">
-        <v>496</v>
+        <v>515</v>
       </c>
       <c r="C258" t="n">
         <v>-2.23042604166836</v>
@@ -7190,10 +7297,10 @@
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>497</v>
+        <v>516</v>
       </c>
       <c r="B259" t="s">
-        <v>498</v>
+        <v>517</v>
       </c>
       <c r="C259" t="n">
         <v>-0.57218573185137</v>
@@ -7210,10 +7317,10 @@
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>499</v>
+        <v>518</v>
       </c>
       <c r="B260" t="s">
-        <v>500</v>
+        <v>519</v>
       </c>
       <c r="C260" t="n">
         <v>-0.92685567996832</v>
@@ -7230,10 +7337,10 @@
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="B261" t="s">
-        <v>502</v>
+        <v>521</v>
       </c>
       <c r="C261" t="n">
         <v>-1.25825150670802</v>
@@ -7250,10 +7357,10 @@
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>503</v>
+        <v>522</v>
       </c>
       <c r="B262" t="s">
-        <v>504</v>
+        <v>523</v>
       </c>
       <c r="C262" t="n">
         <v>3.00958676038468</v>
@@ -7270,10 +7377,10 @@
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>505</v>
+        <v>524</v>
       </c>
       <c r="B263" t="s">
-        <v>506</v>
+        <v>525</v>
       </c>
       <c r="C263" t="n">
         <v>1.58658176380356</v>
@@ -7290,10 +7397,10 @@
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>507</v>
+        <v>526</v>
       </c>
       <c r="B264" t="s">
-        <v>508</v>
+        <v>527</v>
       </c>
       <c r="C264" t="n">
         <v>-0.718886424243888</v>
@@ -7310,10 +7417,10 @@
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>509</v>
+        <v>528</v>
       </c>
       <c r="B265" t="s">
-        <v>510</v>
+        <v>529</v>
       </c>
       <c r="C265" t="n">
         <v>2.68418551050861</v>
@@ -7330,10 +7437,10 @@
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>511</v>
+        <v>530</v>
       </c>
       <c r="B266" t="s">
-        <v>512</v>
+        <v>531</v>
       </c>
       <c r="C266" t="n">
         <v>1.62160281717821</v>
@@ -7350,9 +7457,11 @@
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>513</v>
-      </c>
-      <c r="B267"/>
+        <v>532</v>
+      </c>
+      <c r="B267" t="s">
+        <v>533</v>
+      </c>
       <c r="C267" t="n">
         <v>-1.05836042353364</v>
       </c>
@@ -7368,10 +7477,10 @@
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>514</v>
+        <v>534</v>
       </c>
       <c r="B268" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="C268" t="n">
         <v>0.562250045959906</v>
@@ -7388,10 +7497,10 @@
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>516</v>
+        <v>536</v>
       </c>
       <c r="B269" t="s">
-        <v>517</v>
+        <v>537</v>
       </c>
       <c r="C269" t="n">
         <v>-0.25142512279374</v>
@@ -7408,10 +7517,10 @@
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>518</v>
+        <v>538</v>
       </c>
       <c r="B270" t="s">
-        <v>519</v>
+        <v>539</v>
       </c>
       <c r="C270" t="n">
         <v>-0.661044416244937</v>
@@ -7428,10 +7537,10 @@
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="B271" t="s">
-        <v>521</v>
+        <v>541</v>
       </c>
       <c r="C271" t="n">
         <v>0.630402950740229</v>
@@ -7448,10 +7557,10 @@
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>522</v>
+        <v>542</v>
       </c>
       <c r="B272" t="s">
-        <v>523</v>
+        <v>543</v>
       </c>
       <c r="C272" t="n">
         <v>-0.858015660703802</v>
@@ -7468,10 +7577,10 @@
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>524</v>
+        <v>544</v>
       </c>
       <c r="B273" t="s">
-        <v>525</v>
+        <v>545</v>
       </c>
       <c r="C273" t="n">
         <v>-5.45186527272472</v>
@@ -7488,10 +7597,10 @@
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>526</v>
+        <v>546</v>
       </c>
       <c r="B274" t="s">
-        <v>527</v>
+        <v>547</v>
       </c>
       <c r="C274" t="n">
         <v>-0.854161368766534</v>
@@ -7508,10 +7617,10 @@
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>528</v>
+        <v>548</v>
       </c>
       <c r="B275" t="s">
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="C275" t="n">
         <v>0.614964475637325</v>
@@ -7528,10 +7637,10 @@
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="B276" t="s">
-        <v>531</v>
+        <v>551</v>
       </c>
       <c r="C276" t="n">
         <v>-0.430456770838728</v>
@@ -7548,10 +7657,10 @@
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="B277" t="s">
-        <v>533</v>
+        <v>553</v>
       </c>
       <c r="C277" t="n">
         <v>-0.931823456085637</v>
@@ -7568,10 +7677,10 @@
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>534</v>
+        <v>554</v>
       </c>
       <c r="B278" t="s">
-        <v>535</v>
+        <v>555</v>
       </c>
       <c r="C278" t="n">
         <v>-0.899692849431854</v>
@@ -7588,10 +7697,10 @@
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>536</v>
+        <v>556</v>
       </c>
       <c r="B279" t="s">
-        <v>537</v>
+        <v>557</v>
       </c>
       <c r="C279" t="n">
         <v>2.59718396433158</v>
@@ -7608,10 +7717,10 @@
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>538</v>
+        <v>558</v>
       </c>
       <c r="B280" t="s">
-        <v>539</v>
+        <v>559</v>
       </c>
       <c r="C280" t="n">
         <v>0.482953096249909</v>
@@ -7628,10 +7737,10 @@
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="B281" t="s">
-        <v>541</v>
+        <v>561</v>
       </c>
       <c r="C281" t="n">
         <v>-0.508367751056144</v>
@@ -7648,10 +7757,10 @@
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>542</v>
+        <v>562</v>
       </c>
       <c r="B282" t="s">
-        <v>543</v>
+        <v>563</v>
       </c>
       <c r="C282" t="n">
         <v>0.956574161231153</v>
@@ -7668,9 +7777,11 @@
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>544</v>
-      </c>
-      <c r="B283"/>
+        <v>564</v>
+      </c>
+      <c r="B283" t="s">
+        <v>565</v>
+      </c>
       <c r="C283" t="n">
         <v>1.87966929620981</v>
       </c>
@@ -7686,7 +7797,7 @@
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>545</v>
+        <v>566</v>
       </c>
       <c r="B284"/>
       <c r="C284" t="n">
@@ -7704,10 +7815,10 @@
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>546</v>
+        <v>567</v>
       </c>
       <c r="B285" t="s">
-        <v>547</v>
+        <v>568</v>
       </c>
       <c r="C285" t="n">
         <v>-1.56091300067851</v>
@@ -7724,10 +7835,10 @@
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>548</v>
+        <v>569</v>
       </c>
       <c r="B286" t="s">
-        <v>549</v>
+        <v>570</v>
       </c>
       <c r="C286" t="n">
         <v>-0.974118583117074</v>
@@ -7744,10 +7855,10 @@
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>550</v>
+        <v>571</v>
       </c>
       <c r="B287" t="s">
-        <v>551</v>
+        <v>572</v>
       </c>
       <c r="C287" t="n">
         <v>1.10528948654768</v>
@@ -7764,10 +7875,10 @@
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>552</v>
+        <v>573</v>
       </c>
       <c r="B288" t="s">
-        <v>553</v>
+        <v>574</v>
       </c>
       <c r="C288" t="n">
         <v>2.19175567037061</v>
@@ -7784,10 +7895,10 @@
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>554</v>
+        <v>575</v>
       </c>
       <c r="B289" t="s">
-        <v>555</v>
+        <v>576</v>
       </c>
       <c r="C289" t="n">
         <v>-5.67821160419262</v>
@@ -7804,10 +7915,10 @@
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>556</v>
+        <v>577</v>
       </c>
       <c r="B290" t="s">
-        <v>557</v>
+        <v>578</v>
       </c>
       <c r="C290" t="n">
         <v>1.01184926230506</v>
@@ -7824,10 +7935,10 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>558</v>
+        <v>579</v>
       </c>
       <c r="B291" t="s">
-        <v>559</v>
+        <v>580</v>
       </c>
       <c r="C291" t="n">
         <v>-1.14284770033031</v>
@@ -7844,7 +7955,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>560</v>
+        <v>581</v>
       </c>
       <c r="B292"/>
       <c r="C292" t="n">
@@ -7862,9 +7973,11 @@
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>561</v>
-      </c>
-      <c r="B293"/>
+        <v>582</v>
+      </c>
+      <c r="B293" t="s">
+        <v>583</v>
+      </c>
       <c r="C293" t="n">
         <v>-0.683172203176056</v>
       </c>
@@ -7880,10 +7993,10 @@
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>562</v>
+        <v>584</v>
       </c>
       <c r="B294" t="s">
-        <v>563</v>
+        <v>585</v>
       </c>
       <c r="C294" t="n">
         <v>1.12228893521323</v>
@@ -7900,10 +8013,10 @@
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>564</v>
+        <v>586</v>
       </c>
       <c r="B295" t="s">
-        <v>565</v>
+        <v>587</v>
       </c>
       <c r="C295" t="n">
         <v>-0.922856337531467</v>
@@ -7920,9 +8033,11 @@
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>566</v>
-      </c>
-      <c r="B296"/>
+        <v>588</v>
+      </c>
+      <c r="B296" t="s">
+        <v>589</v>
+      </c>
       <c r="C296" t="n">
         <v>-0.559457192975431</v>
       </c>
@@ -7938,10 +8053,10 @@
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>567</v>
+        <v>590</v>
       </c>
       <c r="B297" t="s">
-        <v>568</v>
+        <v>591</v>
       </c>
       <c r="C297" t="n">
         <v>1.17329072974604</v>
@@ -7958,10 +8073,10 @@
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>569</v>
+        <v>592</v>
       </c>
       <c r="B298" t="s">
-        <v>570</v>
+        <v>593</v>
       </c>
       <c r="C298" t="n">
         <v>1.35366976980453</v>
@@ -7978,10 +8093,10 @@
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>571</v>
+        <v>594</v>
       </c>
       <c r="B299" t="s">
-        <v>572</v>
+        <v>595</v>
       </c>
       <c r="C299" t="n">
         <v>1.00098709267273</v>
@@ -7998,10 +8113,10 @@
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>573</v>
+        <v>596</v>
       </c>
       <c r="B300" t="s">
-        <v>574</v>
+        <v>597</v>
       </c>
       <c r="C300" t="n">
         <v>1.37663103372167</v>
@@ -8018,10 +8133,10 @@
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>575</v>
+        <v>598</v>
       </c>
       <c r="B301" t="s">
-        <v>576</v>
+        <v>599</v>
       </c>
       <c r="C301" t="n">
         <v>-1.01665878449352</v>

</xml_diff>